<commit_message>
updated some topics of the project
</commit_message>
<xml_diff>
--- a/dataset/SaldoAnterior.xlsx
+++ b/dataset/SaldoAnterior.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuário\Documents\_rma\_tecnologia\_data\evolve_data\projetos\projeto_fluxo_de_caixa_evolve\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEC287F-E488-434C-B0E0-BB65ABBEBEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD742D2-1F4C-4B49-8FDF-141E66B1ADC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{69803419-23F1-49B4-B88F-0AA51EE3DECF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{69803419-23F1-49B4-B88F-0AA51EE3DECF}"/>
   </bookViews>
   <sheets>
     <sheet name="SaldoAnterior" sheetId="4" r:id="rId1"/>
@@ -238,11 +238,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -600,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4A0BFC-FEEB-439A-A140-FEB0B86E903E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -654,7 +654,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD75F9D0-C229-48DC-8F29-4F1CE123AC95}">
   <dimension ref="B2:D6"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -663,18 +665,18 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:4">
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:4">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>